<commit_message>
Adding download buttons for results
</commit_message>
<xml_diff>
--- a/ELEphanT/EasyLanguageEvaluationTool/Easy_Language_Reference_Texts.xlsx
+++ b/ELEphanT/EasyLanguageEvaluationTool/Easy_Language_Reference_Texts.xlsx
@@ -43,13 +43,13 @@
             <text:p>Text(s)</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="Default" office:value-type="string" calcext:value-type="string">
-            <text:p>Unweighted</text:p>
+            <text:p>Unweighted Score</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="Default" office:value-type="string" calcext:value-type="string">
-            <text:p>Weighted</text:p>
+            <text:p>Weighted Score</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="Default" office:value-type="string" calcext:value-type="string">
-            <text:p>Perfect Sentences</text:p>
+            <text:p>Amount of Perfect Sentences</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -91,11 +91,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2022-12-02T20:17:11.411406990</meta:creation-date>
-    <dc:date>2022-12-02T20:23:31.223626128</dc:date>
-    <meta:editing-duration>PT6M20S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
+    <dc:date>2022-12-13T10:36:25.806074940</dc:date>
+    <meta:editing-duration>PT6M32S</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
+    <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="12" meta:object-count="0"/>
-    <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
   </office:meta>
 </office:document-meta>
 </file>
@@ -114,7 +114,7 @@
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -128,7 +128,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">852</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1775</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">120</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -173,9 +173,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">XP-235-Series</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lgH+/1hQLTIzNS1TZXJpZXMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpYUC0yMzUtU2VyaWVzAAAAAAAAAAAAAAAAAAAWAAMAswAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9WFAtMjM1LVNlcmllcwpvcmllbnRhdGlvbj1Qb3J0cmFpdApjb3BpZXM9MQpjb2xsYXRlPWZhbHNlCm1hcmdpbmFkanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MQpjb2xvcmRldmljZT0wClBQRENvbnRleHREYXRhClBhZ2VTaXplOkE0AAASAENPTVBBVF9EVVBMRVhfTU9ERRMARHVwbGV4TW9kZTo6VW5rbm93bg==</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -187,6 +187,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="Sheet1">

</xml_diff>